<commit_message>
Changed testing matrix lab4
</commit_message>
<xml_diff>
--- a/downloads/testing matrix.xlsx
+++ b/downloads/testing matrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzapata\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzapata\Documents\GitHub\networkingworkshop\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Lab1 " sheetId="8" r:id="rId1"/>
@@ -324,21 +324,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -355,6 +340,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -683,22 +683,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
         <v>2</v>
@@ -712,26 +712,26 @@
       <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="21"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="21"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -740,11 +740,11 @@
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -753,11 +753,11 @@
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -766,11 +766,11 @@
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
@@ -779,11 +779,11 @@
       <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="26"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -812,22 +812,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
         <v>2</v>
@@ -841,26 +841,26 @@
       <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="21"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="21"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -869,17 +869,17 @@
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="24" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -890,17 +890,17 @@
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="25" t="s">
+      <c r="C5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>12</v>
       </c>
     </row>
@@ -911,17 +911,17 @@
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="24" t="s">
+      <c r="C6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -932,17 +932,17 @@
       <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24" t="s">
+      <c r="C7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -973,23 +973,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="13"/>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
         <v>2</v>
@@ -1006,29 +1006,29 @@
       <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1037,12 +1037,12 @@
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1051,12 +1051,12 @@
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1065,12 +1065,12 @@
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1079,12 +1079,12 @@
       <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
@@ -1093,12 +1093,12 @@
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="26"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1127,23 +1127,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="13"/>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
         <v>2</v>
@@ -1160,29 +1160,29 @@
       <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1191,20 +1191,20 @@
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="24" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1215,20 +1215,20 @@
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="25" t="s">
+      <c r="C5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1239,20 +1239,20 @@
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="24" t="s">
+      <c r="C6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1263,20 +1263,20 @@
       <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="24" t="s">
+      <c r="C7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1287,20 +1287,20 @@
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24" t="s">
+      <c r="C8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1331,23 +1331,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="13"/>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
         <v>2</v>
@@ -1364,29 +1364,29 @@
       <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1395,12 +1395,12 @@
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1409,12 +1409,12 @@
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1423,12 +1423,12 @@
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1437,12 +1437,12 @@
       <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
@@ -1451,12 +1451,12 @@
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="26"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1485,23 +1485,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="13"/>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
         <v>2</v>
@@ -1518,29 +1518,29 @@
       <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1549,20 +1549,20 @@
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="24" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1573,20 +1573,20 @@
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="25" t="s">
+      <c r="C5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1597,20 +1597,20 @@
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="24" t="s">
+      <c r="C6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1621,20 +1621,20 @@
       <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="25" t="s">
+      <c r="C7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1645,20 +1645,20 @@
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="25" t="s">
+      <c r="C8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24" t="s">
+      <c r="G8" s="18"/>
+      <c r="H8" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1689,24 +1689,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
         <v>2</v>
@@ -1726,32 +1726,32 @@
       <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="21"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="21"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1760,13 +1760,13 @@
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1775,13 +1775,13 @@
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1790,13 +1790,13 @@
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1805,13 +1805,13 @@
       <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:9" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1820,13 +1820,13 @@
       <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:9" s="7" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -1835,16 +1835,16 @@
       <c r="B9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="26"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="27"/>
+      <c r="D10" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1861,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1873,24 +1873,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
         <v>2</v>
@@ -1910,32 +1910,32 @@
       <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="21"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="21"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1944,23 +1944,23 @@
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="24" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1971,23 +1971,23 @@
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="25" t="s">
+      <c r="C5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="20" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1998,23 +1998,23 @@
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="24" t="s">
+      <c r="C6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2025,23 +2025,23 @@
       <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="25" t="s">
+      <c r="C7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="24" t="s">
+      <c r="H7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2052,23 +2052,23 @@
       <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="25" t="s">
+      <c r="C8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="24" t="s">
+      <c r="G8" s="18"/>
+      <c r="H8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2079,23 +2079,23 @@
       <c r="B9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24" t="s">
+      <c r="C9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>